<commit_message>
new data dead trees
</commit_message>
<xml_diff>
--- a/data-raw/forestindicators_example_input.xlsx
+++ b/data-raw/forestindicators_example_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gencat.sharepoint.com/sites/CTFC_NAquilu/Documents compartits/General/COLLABORATIONS/EMF/forestindicators/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_0AD5B693B5A585BF0563007530E656F7AA98BCD0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58CF6457-BF94-479F-8A0B-69D44241C71D}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_0AD5B693B5A585BF0563007530E656F7AA98BCD0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F1B1963-FA67-4C21-8344-575A4A9DDD92}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="29">
   <si>
     <t>id_stand</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>cut</t>
+  </si>
+  <si>
+    <t>dead</t>
   </si>
 </sst>
 </file>
@@ -386,11 +389,11 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B10" ca="1" si="0">+ROUND(RAND()*1000, 1)</f>
-        <v>503.1</v>
+        <v>14.3</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C10" ca="1" si="1">+ROUND(RAND()*10, 1)</f>
-        <v>5.9</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -399,11 +402,11 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>661</v>
+        <v>362.6</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -412,11 +415,11 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>986.9</v>
+        <v>319.60000000000002</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2999999999999998</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -425,11 +428,11 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>455</v>
+        <v>635.20000000000005</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -438,11 +441,11 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>670.4</v>
+        <v>774.8</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -451,11 +454,11 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>674</v>
+        <v>166.6</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -464,11 +467,11 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>399.1</v>
+        <v>368</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>9.9</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -477,11 +480,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>550.9</v>
+        <v>945.9</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -490,11 +493,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>724.7</v>
+        <v>548.9</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3</v>
+        <v>1.4</v>
       </c>
     </row>
   </sheetData>
@@ -539,11 +542,11 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C28" ca="1" si="0">+ROUND(RAND()*1000, 1)</f>
-        <v>503.8</v>
+        <v>353.2</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D28" ca="1" si="1">+ROUND(RAND()*100, 1)</f>
-        <v>68.5</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -555,11 +558,11 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6</v>
+        <v>355.1</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>11.3</v>
+        <v>63.2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -571,11 +574,11 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>341.3</v>
+        <v>377</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>43.6</v>
+        <v>68.900000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -587,11 +590,11 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>502.6</v>
+        <v>836.6</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>80.400000000000006</v>
+        <v>24.8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -603,11 +606,11 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>878.2</v>
+        <v>742.4</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>45.4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -619,11 +622,11 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>511.3</v>
+        <v>405.7</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -635,11 +638,11 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>259.8</v>
+        <v>103.3</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -651,11 +654,11 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>305.89999999999998</v>
+        <v>561.79999999999995</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>93.6</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -667,11 +670,11 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>966.3</v>
+        <v>522.1</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>33.6</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -683,11 +686,11 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>489.8</v>
+        <v>383.2</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>95.4</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -699,11 +702,11 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>958.2</v>
+        <v>511.2</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>65.099999999999994</v>
+        <v>85.9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -715,11 +718,11 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>262.3</v>
+        <v>552</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>60.5</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -731,11 +734,11 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>277.7</v>
+        <v>813.3</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>62.5</v>
+        <v>32.9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -747,11 +750,11 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>800.7</v>
+        <v>368</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>49.5</v>
+        <v>50.7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -763,11 +766,11 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>230.6</v>
+        <v>436.1</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>24.4</v>
+        <v>30.2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -779,11 +782,11 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>497.2</v>
+        <v>867.9</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>61.9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -795,11 +798,11 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>868</v>
+        <v>304.60000000000002</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>75.2</v>
+        <v>85.8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -811,11 +814,11 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>13.3</v>
+        <v>349.1</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>67.8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -827,11 +830,11 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>881</v>
+        <v>46.3</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>45.2</v>
+        <v>44.1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -843,11 +846,11 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>200.2</v>
+        <v>335.6</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1</v>
+        <v>33.1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -859,11 +862,11 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>460.2</v>
+        <v>509.6</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -875,11 +878,11 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>530.20000000000005</v>
+        <v>824.6</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>99.6</v>
+        <v>59.1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -891,11 +894,11 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>607.5</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>72.5</v>
+        <v>76.7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -907,11 +910,11 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>514.79999999999995</v>
+        <v>554.79999999999995</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>9.4</v>
+        <v>57.4</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -923,11 +926,11 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>614.5</v>
+        <v>710.4</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>98.6</v>
+        <v>43.8</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -939,11 +942,11 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="0"/>
-        <v>876</v>
+        <v>111.7</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -955,11 +958,11 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="0"/>
-        <v>728.8</v>
+        <v>623.20000000000005</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>59.5</v>
+        <v>12.1</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +1004,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C14" ca="1" si="0">+ROUND(RAND(), 2)</f>
-        <v>0.48</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1013,7 +1016,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1025,7 +1028,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15</v>
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1037,7 +1040,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1049,7 +1052,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1061,7 +1064,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.03</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1073,7 +1076,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1085,7 +1088,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1097,7 +1100,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1109,7 +1112,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57999999999999996</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1121,7 +1124,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1133,7 +1136,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1145,7 +1148,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83</v>
+        <v>0.43</v>
       </c>
     </row>
   </sheetData>
@@ -1156,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1205,15 +1208,15 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E35" ca="1" si="0">+ROUND(RAND()*50, 1)+5</f>
-        <v>30.4</v>
+        <v>18.3</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F35" ca="1" si="1">+ROUND(RAND()*20, 1)+3</f>
-        <v>11.3</v>
+        <v>22.3</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G35" ca="1" si="2">+ROUND(RAND()*1000, 0)</f>
-        <v>457</v>
+        <f t="shared" ref="G2:G26" ca="1" si="2">+ROUND(RAND()*1000, 0)</f>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1231,15 +1234,15 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>28.3</v>
+        <v>36.5</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>12.9</v>
+        <v>18.8</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="2"/>
-        <v>609</v>
+        <v>891</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1257,15 +1260,15 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>25.5</v>
+        <v>51.1</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>20.2</v>
+        <v>5.3</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="2"/>
-        <v>281</v>
+        <v>644</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1283,15 +1286,15 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>13.1</v>
+        <v>36.9</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
-        <v>12.7</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="2"/>
-        <v>803</v>
+        <v>543</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1309,15 +1312,15 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>17.3</v>
+        <v>13.9</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
-        <v>17.5</v>
+        <v>13.3</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="2"/>
-        <v>526</v>
+        <v>852</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1335,15 +1338,15 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>43.7</v>
+        <v>49.1</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>9.9</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="2"/>
-        <v>791</v>
+        <v>698</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1361,15 +1364,15 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>34.799999999999997</v>
+        <v>24.4</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="2"/>
-        <v>703</v>
+        <v>885</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1387,15 +1390,15 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>11.7</v>
+        <v>10.1</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="2"/>
-        <v>200</v>
+        <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1413,15 +1416,15 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>24.9</v>
+        <v>45.3</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="1"/>
-        <v>14.6</v>
+        <v>20.6</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="2"/>
-        <v>506</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1439,15 +1442,15 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>52.2</v>
+        <v>35.1</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="1"/>
-        <v>16.5</v>
+        <v>22.5</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="2"/>
-        <v>850</v>
+        <v>651</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1465,15 +1468,15 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>49.6</v>
+        <v>49.8</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
-        <v>20.7</v>
+        <v>13.6</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="2"/>
-        <v>679</v>
+        <v>424</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1491,15 +1494,15 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>22.7</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
-        <v>19.399999999999999</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="2"/>
-        <v>152</v>
+        <v>506</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1517,15 +1520,15 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>36.9</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
-        <v>13.3</v>
+        <v>6.4</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="2"/>
-        <v>553</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1543,15 +1546,15 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>25.8</v>
+        <v>9.1</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>15.5</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="2"/>
-        <v>695</v>
+        <v>445</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1569,15 +1572,15 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>35.799999999999997</v>
+        <v>41.2</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="1"/>
-        <v>5.4</v>
+        <v>9.6</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="2"/>
-        <v>83</v>
+        <v>851</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1595,15 +1598,15 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>34.1</v>
+        <v>22.4</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="2"/>
-        <v>553</v>
+        <v>491</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1621,15 +1624,15 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8000000000000007</v>
+        <v>5.8</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>565</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1647,15 +1650,15 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>40.9</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>20.5</v>
+        <v>11.7</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="2"/>
-        <v>912</v>
+        <v>433</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1673,15 +1676,15 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>11.6</v>
+        <v>44.8</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>15.5</v>
+        <v>22.7</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="2"/>
-        <v>544</v>
+        <v>576</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1699,15 +1702,15 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>54.3</v>
+        <v>33.1</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>16.8</v>
+        <v>13.1</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="2"/>
-        <v>561</v>
+        <v>769</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1725,15 +1728,15 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>47.8</v>
+        <v>13.9</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>19.600000000000001</v>
+        <v>21.3</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="2"/>
-        <v>902</v>
+        <v>904</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1751,11 +1754,11 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>27.4</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5</v>
+        <v>22.5</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="2"/>
@@ -1777,15 +1780,15 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>53.6</v>
+        <v>19.5</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>19.600000000000001</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="2"/>
-        <v>543</v>
+        <v>818</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1803,15 +1806,15 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>13.8</v>
+        <v>12</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="2"/>
-        <v>464</v>
+        <v>592</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1829,15 +1832,15 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>35.799999999999997</v>
+        <v>11.2</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>22.1</v>
+        <v>12.5</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>357</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1855,15 +1858,15 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>27.2</v>
+        <v>43.9</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>19.8</v>
+        <v>18.3</v>
       </c>
       <c r="G27">
         <f ca="1">+ROUND(RAND()*200, 0)</f>
-        <v>120</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1881,15 +1884,15 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>41.4</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>19.2</v>
+        <v>3.5</v>
       </c>
       <c r="G28">
         <f t="shared" ref="G28:G35" ca="1" si="3">+ROUND(RAND()*200, 0)</f>
-        <v>6</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1907,15 +1910,15 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>24.8</v>
+        <v>29.1</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="3"/>
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1933,15 +1936,15 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>18.899999999999999</v>
+        <v>49.4</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3</v>
+        <v>5.8</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="3"/>
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1959,15 +1962,15 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7</v>
+        <v>13</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="3"/>
-        <v>182</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1985,15 +1988,15 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>54.1</v>
+        <v>17.2</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2</v>
+        <v>20.6</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -2011,15 +2014,15 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F33">
         <f t="shared" ca="1" si="1"/>
-        <v>19.899999999999999</v>
+        <v>4.3</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="3"/>
-        <v>108</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2037,15 +2040,15 @@
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="0"/>
-        <v>19.399999999999999</v>
+        <v>44.1</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4</v>
+        <v>7.1</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="3"/>
-        <v>73</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2063,15 +2066,275 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="0"/>
-        <v>27.9</v>
+        <v>45.7</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="1"/>
-        <v>12.2</v>
+        <v>11.8</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="2">
+        <v>45717</v>
+      </c>
+      <c r="D36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ref="E36:E45" ca="1" si="4">+ROUND(RAND()*50, 1)+5</f>
+        <v>26.1</v>
+      </c>
+      <c r="F36">
+        <f ca="1">+ROUND(RAND()*20, 1)</f>
+        <v>13.3</v>
+      </c>
+      <c r="G36">
+        <f ca="1">+ROUND(RAND()*100, 0)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="2">
+        <v>45717</v>
+      </c>
+      <c r="D37" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37">
+        <f t="shared" ca="1" si="4"/>
+        <v>36.200000000000003</v>
+      </c>
+      <c r="F37">
+        <f t="shared" ref="F37:F45" ca="1" si="5">+ROUND(RAND()*20, 1)</f>
+        <v>11</v>
+      </c>
+      <c r="G37">
+        <f t="shared" ref="G37:G45" ca="1" si="6">+ROUND(RAND()*100, 0)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="2">
+        <v>45717</v>
+      </c>
+      <c r="D38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38">
+        <f t="shared" ca="1" si="4"/>
+        <v>49.6</v>
+      </c>
+      <c r="F38">
+        <f t="shared" ca="1" si="5"/>
+        <v>6.9</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ca="1" si="6"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="2">
+        <v>45717</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ca="1" si="4"/>
+        <v>40.5</v>
+      </c>
+      <c r="F39">
+        <f t="shared" ca="1" si="5"/>
+        <v>10.9</v>
+      </c>
+      <c r="G39">
+        <f t="shared" ca="1" si="6"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="2">
+        <v>45658</v>
+      </c>
+      <c r="D40" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40">
+        <f t="shared" ca="1" si="4"/>
+        <v>25.9</v>
+      </c>
+      <c r="F40">
+        <f t="shared" ca="1" si="5"/>
+        <v>7.7</v>
+      </c>
+      <c r="G40">
+        <f t="shared" ca="1" si="6"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="2">
+        <v>45658</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41">
+        <f t="shared" ca="1" si="4"/>
+        <v>18.7</v>
+      </c>
+      <c r="F41">
+        <f t="shared" ca="1" si="5"/>
+        <v>13.4</v>
+      </c>
+      <c r="G41">
+        <f t="shared" ca="1" si="6"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45658</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ca="1" si="4"/>
+        <v>16.7</v>
+      </c>
+      <c r="F42">
+        <f t="shared" ca="1" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="G42">
+        <f t="shared" ca="1" si="6"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="2">
+        <v>45689</v>
+      </c>
+      <c r="D43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ca="1" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="F43">
+        <f t="shared" ca="1" si="5"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G43">
+        <f t="shared" ca="1" si="6"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="2">
+        <v>45717</v>
+      </c>
+      <c r="D44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44">
+        <f t="shared" ca="1" si="4"/>
+        <v>35.1</v>
+      </c>
+      <c r="F44">
+        <f t="shared" ca="1" si="5"/>
+        <v>2.5</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ca="1" si="6"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="2">
+        <v>45717</v>
+      </c>
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45">
+        <f t="shared" ca="1" si="4"/>
+        <v>7.1</v>
+      </c>
+      <c r="F45">
+        <f t="shared" ca="1" si="5"/>
+        <v>7.6</v>
+      </c>
+      <c r="G45">
+        <f t="shared" ca="1" si="6"/>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2081,8 +2344,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010095DDF5E8B92F09488F6994CC76A3261F" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="17c4366f67cb7703288c6b086a65acc2">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="10b2415f-6b16-408d-a5df-bf55a3837e9c" xmlns:ns3="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a91d07ec0072abfb5523443b79ceeaf" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="10b2415f-6b16-408d-a5df-bf55a3837e9c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095DDF5E8B92F09488F6994CC76A3261F" ma:contentTypeVersion="14" ma:contentTypeDescription="Crea un document nou" ma:contentTypeScope="" ma:versionID="77fb5a445c241a114a6db4ced5f4c9a2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="10b2415f-6b16-408d-a5df-bf55a3837e9c" xmlns:ns3="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a9fed371820f3b6ac84a8d3142ba9e2" ns2:_="" ns3:_="">
     <xsd:import namespace="10b2415f-6b16-408d-a5df-bf55a3837e9c"/>
     <xsd:import namespace="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8"/>
     <xsd:element name="properties">
@@ -2134,7 +2417,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="d19f90c4-00d9-45b7-bc62-04f95cbe7a8b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetes de la imatge" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="d19f90c4-00d9-45b7-bc62-04f95cbe7a8b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -2203,8 +2486,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipus de contingut"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Títol"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -2293,34 +2576,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="10b2415f-6b16-408d-a5df-bf55a3837e9c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6988A91E-D8FE-4922-8072-A14B3A4234FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8126180-C4CE-4F4C-B877-9355FC3468E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8"/>
+    <ds:schemaRef ds:uri="10b2415f-6b16-408d-a5df-bf55a3837e9c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DF7B23B-9604-45E2-8F86-2CB9E5DF60B1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DF7B23B-9604-45E2-8F86-2CB9E5DF60B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8126180-C4CE-4F4C-B877-9355FC3468E5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED2FFE9-E376-437F-876C-4A93A3F7AA43}"/>
 </file>
</xml_diff>

<commit_message>
new funding project in README
</commit_message>
<xml_diff>
--- a/data-raw/forestindicators_example_input.xlsx
+++ b/data-raw/forestindicators_example_input.xlsx
@@ -2643,6 +2643,239 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010095DDF5E8B92F09488F6994CC76A3261F" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c83b49f018a59e932b4bb22d3a3baca6">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="10b2415f-6b16-408d-a5df-bf55a3837e9c" xmlns:ns3="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0570fb1bd9374cf929842058f023efb" ns2:_="" ns3:_="">
+    <xsd:import namespace="10b2415f-6b16-408d-a5df-bf55a3837e9c"/>
+    <xsd:import namespace="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="10b2415f-6b16-408d-a5df-bf55a3837e9c" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="d19f90c4-00d9-45b7-bc62-04f95cbe7a8b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:description="" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="21" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{cebcb379-39a5-4efc-8079-d623ba702961}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="10b2415f-6b16-408d-a5df-bf55a3837e9c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="cb52536f-ae72-4a59-84ed-2e4ff2cac1d8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8126180-C4CE-4F4C-B877-9355FC3468E5}">
   <ds:schemaRefs>
@@ -2664,4 +2897,16 @@
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED2FFE9-E376-437F-876C-4A93A3F7AA43}"/>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AF1B8B4-3FB1-4F40-AA1F-B4CCB19EF01D}"/>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B7703DB-4CCC-4AF9-AE39-47A31EAC3E43}"/>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2558CD12-3729-44E6-B11E-6A1DCA8FCDF5}"/>
 </file>
</xml_diff>